<commit_message>
b2b done in test.py
</commit_message>
<xml_diff>
--- a/B2BExample.xlsx
+++ b/B2BExample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CLAUDIA\Desktop\DavidC\vsprojects\PhotoManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD63E12-E25A-44C3-AE39-265EEA982712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{86DA9DF8-0579-4F23-8648-4B58D3583E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2692,15 +2692,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2708,30 +2700,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3072,13 +3040,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN376"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AC3" sqref="AC3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="30.3984375" bestFit="1" customWidth="1"/>
-    <col min="25" max="28" width="0" hidden="1" customWidth="1"/>
+    <col min="25" max="28" width="11.19921875" customWidth="1"/>
+    <col min="36" max="36" width="20.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.3">
@@ -31303,7 +31274,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>